<commit_message>
add chrome headless in the project and run the test cases in parallel throug the testng.xml file
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASMAA ASHRAF\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACA08CB-57F9-4B90-8942-500CDBD828E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF57C6F5-70BB-4FA0-83FC-269C5C0D57C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterUsersData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
     <t>FirstName</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>OldQuantity</t>
-  </si>
-  <si>
-    <t>3rd Album</t>
-  </si>
-  <si>
-    <t>3rd</t>
   </si>
   <si>
     <t>Egypt</t>
@@ -488,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,20 +515,6 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -770,10 +750,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91076A63-3F02-47E0-8900-10BD45A2B785}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,14 +777,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -814,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -837,7 +809,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>123456789</v>
+        <v>1234567</v>
       </c>
     </row>
   </sheetData>
@@ -850,10 +822,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -873,11 +845,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -885,7 +852,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04F0911-0F85-442D-921C-33BDFADD1D80}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -914,14 +881,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -929,7 +888,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F901BD-24CA-49C6-B1E5-D5DABC4FC45D}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -948,11 +907,6 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1017,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49E34D4-D80B-4A0B-B43C-36333F2B2ED8}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1084,7 +1038,7 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -1163,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F02C73-25F0-4133-945D-40B22FEBF0E8}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1205,20 +1159,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>